<commit_message>
Added function for printing degrees of each node and added SDN data
</commit_message>
<xml_diff>
--- a/iso3CountryCoordinates.xlsx
+++ b/iso3CountryCoordinates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16900" yWindow="460" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="iso3CountryCoordinates" sheetId="1" r:id="rId1"/>
@@ -932,9 +932,6 @@
     <t>SDN</t>
   </si>
   <si>
-    <t>Sudan</t>
-  </si>
-  <si>
     <t>SUR</t>
   </si>
   <si>
@@ -1200,6 +1197,9 @@
   </si>
   <si>
     <t>Lao PDR</t>
+  </si>
+  <si>
+    <t>Fm Sudan</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1688,7 +1688,7 @@
         <v>-77.396280000000004</v>
       </c>
       <c r="D12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1917,7 +1917,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B29">
         <v>15.120142</v>
@@ -1926,7 +1926,7 @@
         <v>-23.605172100000001</v>
       </c>
       <c r="D29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
         <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2083,7 +2083,7 @@
         <v>15.827659000000001</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2158,7 +2158,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B46">
         <v>7.5399890000000003</v>
@@ -2167,7 +2167,7 @@
         <v>-5.5470800000000002</v>
       </c>
       <c r="D46" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2251,7 +2251,7 @@
         <v>30.802498</v>
       </c>
       <c r="D52" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>100</v>
       </c>
       <c r="E54" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2324,7 +2324,7 @@
         <v>40.489673000000003</v>
       </c>
       <c r="D57" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>-15.310138999999999</v>
       </c>
       <c r="D62" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,12 +2537,12 @@
         <v>134</v>
       </c>
       <c r="E72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B73">
         <v>41.902915999999998</v>
@@ -2551,10 +2551,10 @@
         <v>12.453389</v>
       </c>
       <c r="D73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2638,7 +2638,7 @@
         <v>53.688046</v>
       </c>
       <c r="D79" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2806,7 +2806,7 @@
         <v>74.766098</v>
       </c>
       <c r="D91" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2820,7 +2820,7 @@
         <v>102.495496</v>
       </c>
       <c r="D92" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2879,7 +2879,7 @@
         <v>177</v>
       </c>
       <c r="E96" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2910,7 +2910,7 @@
         <v>181</v>
       </c>
       <c r="E98" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>199</v>
       </c>
       <c r="E107" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3095,7 +3095,7 @@
         <v>150.55081200000001</v>
       </c>
       <c r="D111" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3126,7 +3126,7 @@
         <v>210</v>
       </c>
       <c r="E113" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
         <v>95.956222999999994</v>
       </c>
       <c r="D118" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3227,7 +3227,7 @@
         <v>223</v>
       </c>
       <c r="E120" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3328,7 +3328,7 @@
         <v>237</v>
       </c>
       <c r="E127" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3524,7 +3524,7 @@
         <v>105.31875599999999</v>
       </c>
       <c r="D141" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3552,7 +3552,7 @@
         <v>-62.782997999999999</v>
       </c>
       <c r="D143" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3566,7 +3566,7 @@
         <v>-60.978892999999999</v>
       </c>
       <c r="D144" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -3597,7 +3597,7 @@
         <v>272</v>
       </c>
       <c r="E146" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3611,7 +3611,7 @@
         <v>6.6130810000000002</v>
       </c>
       <c r="D147" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
         <v>279</v>
       </c>
       <c r="E150" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3712,7 +3712,7 @@
         <v>19.699024000000001</v>
       </c>
       <c r="D154" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3757,7 +3757,7 @@
         <v>292</v>
       </c>
       <c r="E157" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3785,12 +3785,12 @@
         <v>127.76692199999999</v>
       </c>
       <c r="D159" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B160">
         <v>4.8593630000000001</v>
@@ -3799,10 +3799,10 @@
         <v>31.571251</v>
       </c>
       <c r="D160" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E160" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -3835,7 +3835,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B163">
         <v>12.984305000000001</v>
@@ -3844,12 +3844,12 @@
         <v>-61.287227999999999</v>
       </c>
       <c r="D163" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B164">
         <v>31.952162000000001</v>
@@ -3858,7 +3858,7 @@
         <v>35.233153999999999</v>
       </c>
       <c r="D164" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3872,12 +3872,12 @@
         <v>30.217635999999999</v>
       </c>
       <c r="D165" t="s">
-        <v>301</v>
+        <v>390</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B166">
         <v>3.919305</v>
@@ -3886,12 +3886,12 @@
         <v>-56.027782999999999</v>
       </c>
       <c r="D166" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B167">
         <v>-26.522503</v>
@@ -3900,12 +3900,12 @@
         <v>31.465865999999998</v>
       </c>
       <c r="D167" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B168">
         <v>60.128160999999999</v>
@@ -3914,12 +3914,12 @@
         <v>18.643501000000001</v>
       </c>
       <c r="D168" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B169">
         <v>46.818187999999999</v>
@@ -3928,12 +3928,12 @@
         <v>8.2275120000000008</v>
       </c>
       <c r="D169" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B170">
         <v>34.802075000000002</v>
@@ -3942,12 +3942,12 @@
         <v>38.996814999999998</v>
       </c>
       <c r="D170" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B171">
         <v>38.861033999999997</v>
@@ -3956,12 +3956,12 @@
         <v>71.276093000000003</v>
       </c>
       <c r="D171" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B172">
         <v>-6.3690280000000001</v>
@@ -3970,12 +3970,12 @@
         <v>34.888821999999998</v>
       </c>
       <c r="D172" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B173">
         <v>41.608635</v>
@@ -3984,12 +3984,12 @@
         <v>21.745274999999999</v>
       </c>
       <c r="D173" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B174">
         <v>15.870032</v>
@@ -3998,12 +3998,12 @@
         <v>100.992541</v>
       </c>
       <c r="D174" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B175">
         <v>-8.8742169999999998</v>
@@ -4012,15 +4012,15 @@
         <v>125.72753899999999</v>
       </c>
       <c r="D175" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E175" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B176">
         <v>8.6195430000000002</v>
@@ -4029,12 +4029,12 @@
         <v>0.82478200000000002</v>
       </c>
       <c r="D176" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B177">
         <v>-21.178985999999998</v>
@@ -4043,12 +4043,12 @@
         <v>-175.19824199999999</v>
       </c>
       <c r="D177" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B178">
         <v>10.691803</v>
@@ -4057,12 +4057,12 @@
         <v>-61.222503000000003</v>
       </c>
       <c r="D178" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B179">
         <v>33.886916999999997</v>
@@ -4071,12 +4071,12 @@
         <v>9.5374990000000004</v>
       </c>
       <c r="D179" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B180">
         <v>38.963745000000003</v>
@@ -4085,12 +4085,12 @@
         <v>35.243321999999999</v>
       </c>
       <c r="D180" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B181">
         <v>38.969718999999998</v>
@@ -4099,12 +4099,12 @@
         <v>59.556277999999999</v>
       </c>
       <c r="D181" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B182">
         <v>-7.1095350000000002</v>
@@ -4113,12 +4113,12 @@
         <v>177.64932999999999</v>
       </c>
       <c r="D182" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B183">
         <v>1.3733329999999999</v>
@@ -4127,12 +4127,12 @@
         <v>32.290275000000001</v>
       </c>
       <c r="D183" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B184">
         <v>48.379432999999999</v>
@@ -4141,12 +4141,12 @@
         <v>31.165579999999999</v>
       </c>
       <c r="D184" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B185">
         <v>23.424075999999999</v>
@@ -4155,12 +4155,12 @@
         <v>53.847817999999997</v>
       </c>
       <c r="D185" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B186">
         <v>55.378050999999999</v>
@@ -4169,12 +4169,12 @@
         <v>-3.4359730000000002</v>
       </c>
       <c r="D186" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B187">
         <v>37.090240000000001</v>
@@ -4183,12 +4183,12 @@
         <v>-95.712890999999999</v>
       </c>
       <c r="D187" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B188">
         <v>-32.522779</v>
@@ -4197,12 +4197,12 @@
         <v>-55.765835000000003</v>
       </c>
       <c r="D188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B189">
         <v>41.377490999999999</v>
@@ -4211,15 +4211,15 @@
         <v>64.585262</v>
       </c>
       <c r="D189" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E189" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B190">
         <v>-15.376706</v>
@@ -4228,12 +4228,12 @@
         <v>166.959158</v>
       </c>
       <c r="D190" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B191">
         <v>6.4237500000000001</v>
@@ -4242,12 +4242,12 @@
         <v>-66.589730000000003</v>
       </c>
       <c r="D191" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B192">
         <v>14.058324000000001</v>
@@ -4256,12 +4256,12 @@
         <v>108.277199</v>
       </c>
       <c r="D192" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B193">
         <v>15.552727000000001</v>
@@ -4270,12 +4270,12 @@
         <v>48.516387999999999</v>
       </c>
       <c r="D193" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B194">
         <v>-13.133896999999999</v>
@@ -4284,12 +4284,12 @@
         <v>27.849332</v>
       </c>
       <c r="D194" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B195">
         <v>-19.015438</v>
@@ -4298,7 +4298,7 @@
         <v>29.154857</v>
       </c>
       <c r="D195" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some missing country data and fixed VCT name in mapping file
</commit_message>
<xml_diff>
--- a/iso3CountryCoordinates.xlsx
+++ b/iso3CountryCoordinates.xlsx
@@ -1109,9 +1109,6 @@
     <t>South Sudan</t>
   </si>
   <si>
-    <t>St. Vincent and Grenadines</t>
-  </si>
-  <si>
     <t>MKD</t>
   </si>
   <si>
@@ -1200,6 +1197,9 @@
   </si>
   <si>
     <t>Fm Sudan</t>
+  </si>
+  <si>
+    <t>St. Vincent and the Grenadines</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1688,7 +1688,7 @@
         <v>-77.396280000000004</v>
       </c>
       <c r="D12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1917,7 +1917,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B29">
         <v>15.120142</v>
@@ -1926,7 +1926,7 @@
         <v>-23.605172100000001</v>
       </c>
       <c r="D29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
         <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2083,7 +2083,7 @@
         <v>15.827659000000001</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2158,7 +2158,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B46">
         <v>7.5399890000000003</v>
@@ -2167,7 +2167,7 @@
         <v>-5.5470800000000002</v>
       </c>
       <c r="D46" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2251,7 +2251,7 @@
         <v>30.802498</v>
       </c>
       <c r="D52" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>100</v>
       </c>
       <c r="E54" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2324,7 +2324,7 @@
         <v>40.489673000000003</v>
       </c>
       <c r="D57" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>-15.310138999999999</v>
       </c>
       <c r="D62" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,12 +2537,12 @@
         <v>134</v>
       </c>
       <c r="E72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B73">
         <v>41.902915999999998</v>
@@ -2554,7 +2554,7 @@
         <v>358</v>
       </c>
       <c r="E73" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2638,7 +2638,7 @@
         <v>53.688046</v>
       </c>
       <c r="D79" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2806,7 +2806,7 @@
         <v>74.766098</v>
       </c>
       <c r="D91" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2820,7 +2820,7 @@
         <v>102.495496</v>
       </c>
       <c r="D92" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2879,7 +2879,7 @@
         <v>177</v>
       </c>
       <c r="E96" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2910,7 +2910,7 @@
         <v>181</v>
       </c>
       <c r="E98" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>199</v>
       </c>
       <c r="E107" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3095,7 +3095,7 @@
         <v>150.55081200000001</v>
       </c>
       <c r="D111" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3126,7 +3126,7 @@
         <v>210</v>
       </c>
       <c r="E113" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
         <v>95.956222999999994</v>
       </c>
       <c r="D118" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3227,7 +3227,7 @@
         <v>223</v>
       </c>
       <c r="E120" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3328,7 +3328,7 @@
         <v>237</v>
       </c>
       <c r="E127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3524,7 +3524,7 @@
         <v>105.31875599999999</v>
       </c>
       <c r="D141" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3552,7 +3552,7 @@
         <v>-62.782997999999999</v>
       </c>
       <c r="D143" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3566,7 +3566,7 @@
         <v>-60.978892999999999</v>
       </c>
       <c r="D144" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -3597,7 +3597,7 @@
         <v>272</v>
       </c>
       <c r="E146" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3611,7 +3611,7 @@
         <v>6.6130810000000002</v>
       </c>
       <c r="D147" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
         <v>279</v>
       </c>
       <c r="E150" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3712,7 +3712,7 @@
         <v>19.699024000000001</v>
       </c>
       <c r="D154" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3757,7 +3757,7 @@
         <v>292</v>
       </c>
       <c r="E157" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3785,12 +3785,12 @@
         <v>127.76692199999999</v>
       </c>
       <c r="D159" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B160">
         <v>4.8593630000000001</v>
@@ -3802,7 +3802,7 @@
         <v>359</v>
       </c>
       <c r="E160" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -3835,7 +3835,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B163">
         <v>12.984305000000001</v>
@@ -3844,12 +3844,12 @@
         <v>-61.287227999999999</v>
       </c>
       <c r="D163" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B164">
         <v>31.952162000000001</v>
@@ -3858,7 +3858,7 @@
         <v>35.233153999999999</v>
       </c>
       <c r="D164" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3872,7 +3872,7 @@
         <v>30.217635999999999</v>
       </c>
       <c r="D165" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3942,7 +3942,7 @@
         <v>38.996814999999998</v>
       </c>
       <c r="D170" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3975,7 +3975,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B173">
         <v>41.608635</v>
@@ -3984,7 +3984,7 @@
         <v>21.745274999999999</v>
       </c>
       <c r="D173" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -4015,7 +4015,7 @@
         <v>317</v>
       </c>
       <c r="E175" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -4214,7 +4214,7 @@
         <v>345</v>
       </c>
       <c r="E189" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Removed disconnected countries (countries lacking data)
</commit_message>
<xml_diff>
--- a/iso3CountryCoordinates.xlsx
+++ b/iso3CountryCoordinates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcmaceac/Documents/School/EECS4414/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\EECS4414\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0906AFE4-8788-475F-A6B3-6F8477DD06F9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="465" windowWidth="24960" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso3CountryCoordinates" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
   <si>
     <t>AFG</t>
   </si>
@@ -248,12 +249,6 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>Congo [DRC]</t>
-  </si>
-  <si>
     <t>COG</t>
   </si>
   <si>
@@ -569,12 +564,6 @@
     <t>Libya</t>
   </si>
   <si>
-    <t>LIE</t>
-  </si>
-  <si>
-    <t>Liechtenstein</t>
-  </si>
-  <si>
     <t>LTU</t>
   </si>
   <si>
@@ -656,12 +645,6 @@
     <t>Moldova</t>
   </si>
   <si>
-    <t>MCO</t>
-  </si>
-  <si>
-    <t>Monaco</t>
-  </si>
-  <si>
     <t>MNG</t>
   </si>
   <si>
@@ -737,12 +720,6 @@
     <t>Nigeria</t>
   </si>
   <si>
-    <t>PRK</t>
-  </si>
-  <si>
-    <t>North Korea</t>
-  </si>
-  <si>
     <t>NOR</t>
   </si>
   <si>
@@ -863,12 +840,6 @@
     <t>Senegal</t>
   </si>
   <si>
-    <t>SRB</t>
-  </si>
-  <si>
-    <t>Serbia</t>
-  </si>
-  <si>
     <t>SYC</t>
   </si>
   <si>
@@ -1128,9 +1099,6 @@
   </si>
   <si>
     <t>CPV</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>Bahamas, The</t>
@@ -1205,7 +1173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1247,6 +1215,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1514,16 +1485,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E195"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="I168" sqref="I168"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1565,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1579,7 +1550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1593,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1607,7 +1578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1621,7 +1592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1677,7 +1648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1688,10 +1659,10 @@
         <v>-77.396280000000004</v>
       </c>
       <c r="D12" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1705,7 +1676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1719,7 +1690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1733,7 +1704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1718,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +1732,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1775,7 +1746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1789,7 +1760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1803,7 +1774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1817,7 +1788,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1831,7 +1802,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1845,7 +1816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1859,7 +1830,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1873,7 +1844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1887,7 +1858,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1901,7 +1872,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1915,9 +1886,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B29">
         <v>15.120142</v>
@@ -1926,10 +1897,10 @@
         <v>-23.605172100000001</v>
       </c>
       <c r="D29" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1943,7 +1914,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1957,7 +1928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1971,7 +1942,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1985,7 +1956,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1999,7 +1970,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2013,7 +1984,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -2027,7 +1998,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -2041,7 +2012,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2055,2250 +2026,2132 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B39" s="1">
-        <v>-4.0383329999999997</v>
+        <v>-0.228021</v>
       </c>
       <c r="C39" s="1">
-        <v>21.758664</v>
+        <v>15.827659000000001</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>74</v>
       </c>
-      <c r="E39" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B40">
+        <v>9.7489170000000005</v>
+      </c>
+      <c r="C40">
+        <v>-83.753428</v>
+      </c>
+      <c r="D40" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="1">
-        <v>-0.228021</v>
-      </c>
-      <c r="C40" s="1">
-        <v>15.827659000000001</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
       <c r="B41">
-        <v>9.7489170000000005</v>
+        <v>45.1</v>
       </c>
       <c r="C41">
-        <v>-83.753428</v>
+        <v>15.2</v>
       </c>
       <c r="D41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
       <c r="B42">
-        <v>45.1</v>
+        <v>21.521757000000001</v>
       </c>
       <c r="C42">
-        <v>15.2</v>
+        <v>-77.781166999999996</v>
       </c>
       <c r="D42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>80</v>
       </c>
       <c r="B43">
-        <v>21.521757000000001</v>
+        <v>35.126412999999999</v>
       </c>
       <c r="C43">
-        <v>-77.781166999999996</v>
+        <v>33.429859</v>
       </c>
       <c r="D43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>82</v>
       </c>
       <c r="B44">
-        <v>35.126412999999999</v>
+        <v>49.817492000000001</v>
       </c>
       <c r="C44">
-        <v>33.429859</v>
+        <v>15.472962000000001</v>
       </c>
       <c r="D44" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>351</v>
+      </c>
+      <c r="B45">
+        <v>7.5399890000000003</v>
+      </c>
+      <c r="C45">
+        <v>-5.5470800000000002</v>
+      </c>
+      <c r="D45" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>84</v>
       </c>
-      <c r="B45">
-        <v>49.817492000000001</v>
-      </c>
-      <c r="C45">
-        <v>15.472962000000001</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B46">
+        <v>56.263919999999999</v>
+      </c>
+      <c r="C46">
+        <v>9.5017849999999999</v>
+      </c>
+      <c r="D46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>361</v>
-      </c>
-      <c r="B46">
-        <v>7.5399890000000003</v>
-      </c>
-      <c r="C46">
-        <v>-5.5470800000000002</v>
-      </c>
-      <c r="D46" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
       <c r="B47">
-        <v>56.263919999999999</v>
+        <v>11.825138000000001</v>
       </c>
       <c r="C47">
-        <v>9.5017849999999999</v>
+        <v>42.590274999999998</v>
       </c>
       <c r="D47" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
       <c r="B48">
-        <v>11.825138000000001</v>
+        <v>15.414999</v>
       </c>
       <c r="C48">
-        <v>42.590274999999998</v>
+        <v>-61.370975999999999</v>
       </c>
       <c r="D48" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>90</v>
       </c>
       <c r="B49">
-        <v>15.414999</v>
+        <v>18.735693000000001</v>
       </c>
       <c r="C49">
-        <v>-61.370975999999999</v>
+        <v>-70.162650999999997</v>
       </c>
       <c r="D49" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>92</v>
       </c>
       <c r="B50">
-        <v>18.735693000000001</v>
+        <v>-1.8312390000000001</v>
       </c>
       <c r="C50">
-        <v>-70.162650999999997</v>
+        <v>-78.183406000000005</v>
       </c>
       <c r="D50" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
       <c r="B51">
-        <v>-1.8312390000000001</v>
+        <v>26.820553</v>
       </c>
       <c r="C51">
-        <v>-78.183406000000005</v>
+        <v>30.802498</v>
       </c>
       <c r="D51" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B52">
+        <v>13.794185000000001</v>
+      </c>
+      <c r="C52">
+        <v>-88.896529999999998</v>
+      </c>
+      <c r="D52" t="s">
         <v>96</v>
       </c>
-      <c r="B52">
-        <v>26.820553</v>
-      </c>
-      <c r="C52">
-        <v>30.802498</v>
-      </c>
-      <c r="D52" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>97</v>
       </c>
       <c r="B53">
-        <v>13.794185000000001</v>
+        <v>1.650801</v>
       </c>
       <c r="C53">
-        <v>-88.896529999999998</v>
+        <v>10.267894999999999</v>
       </c>
       <c r="D53" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>99</v>
       </c>
       <c r="B54">
-        <v>1.650801</v>
+        <v>15.179384000000001</v>
       </c>
       <c r="C54">
-        <v>10.267894999999999</v>
+        <v>39.782333999999999</v>
       </c>
       <c r="D54" t="s">
         <v>100</v>
       </c>
-      <c r="E54" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>101</v>
       </c>
       <c r="B55">
-        <v>15.179384000000001</v>
+        <v>58.595272000000001</v>
       </c>
       <c r="C55">
-        <v>39.782333999999999</v>
+        <v>25.013607</v>
       </c>
       <c r="D55" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>103</v>
       </c>
       <c r="B56">
-        <v>58.595272000000001</v>
+        <v>9.1449999999999996</v>
       </c>
       <c r="C56">
-        <v>25.013607</v>
+        <v>40.489673000000003</v>
       </c>
       <c r="D56" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57">
+        <v>-16.578192999999999</v>
+      </c>
+      <c r="C57">
+        <v>179.414413</v>
+      </c>
+      <c r="D57" t="s">
         <v>105</v>
       </c>
-      <c r="B57">
-        <v>9.1449999999999996</v>
-      </c>
-      <c r="C57">
-        <v>40.489673000000003</v>
-      </c>
-      <c r="D57" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>106</v>
       </c>
       <c r="B58">
-        <v>-16.578192999999999</v>
+        <v>61.924109999999999</v>
       </c>
       <c r="C58">
-        <v>179.414413</v>
+        <v>25.748151</v>
       </c>
       <c r="D58" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>108</v>
       </c>
       <c r="B59">
-        <v>61.924109999999999</v>
+        <v>46.227637999999999</v>
       </c>
       <c r="C59">
-        <v>25.748151</v>
+        <v>2.213749</v>
       </c>
       <c r="D59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>110</v>
       </c>
       <c r="B60">
-        <v>46.227637999999999</v>
+        <v>-0.80368899999999999</v>
       </c>
       <c r="C60">
-        <v>2.213749</v>
+        <v>11.609444</v>
       </c>
       <c r="D60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>112</v>
       </c>
       <c r="B61">
-        <v>-0.80368899999999999</v>
+        <v>13.443182</v>
       </c>
       <c r="C61">
-        <v>11.609444</v>
+        <v>-15.310138999999999</v>
       </c>
       <c r="D61" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>42.315407</v>
+      </c>
+      <c r="C62">
+        <v>43.356892000000002</v>
+      </c>
+      <c r="D62" t="s">
         <v>114</v>
       </c>
-      <c r="B62">
-        <v>13.443182</v>
-      </c>
-      <c r="C62">
-        <v>-15.310138999999999</v>
-      </c>
-      <c r="D62" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>115</v>
       </c>
       <c r="B63">
-        <v>42.315407</v>
+        <v>51.165691000000002</v>
       </c>
       <c r="C63">
-        <v>43.356892000000002</v>
+        <v>10.451525999999999</v>
       </c>
       <c r="D63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>117</v>
       </c>
       <c r="B64">
-        <v>51.165691000000002</v>
+        <v>7.9465269999999997</v>
       </c>
       <c r="C64">
-        <v>10.451525999999999</v>
+        <v>-1.0231939999999999</v>
       </c>
       <c r="D64" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>119</v>
       </c>
       <c r="B65">
-        <v>7.9465269999999997</v>
+        <v>39.074207999999999</v>
       </c>
       <c r="C65">
-        <v>-1.0231939999999999</v>
+        <v>21.824311999999999</v>
       </c>
       <c r="D65" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>121</v>
       </c>
       <c r="B66">
-        <v>39.074207999999999</v>
+        <v>12.262776000000001</v>
       </c>
       <c r="C66">
-        <v>21.824311999999999</v>
+        <v>-61.604171000000001</v>
       </c>
       <c r="D66" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>123</v>
       </c>
       <c r="B67">
-        <v>12.262776000000001</v>
+        <v>15.783471</v>
       </c>
       <c r="C67">
-        <v>-61.604171000000001</v>
+        <v>-90.230759000000006</v>
       </c>
       <c r="D67" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>125</v>
       </c>
       <c r="B68">
-        <v>15.783471</v>
+        <v>9.9455869999999997</v>
       </c>
       <c r="C68">
-        <v>-90.230759000000006</v>
+        <v>-9.6966450000000002</v>
       </c>
       <c r="D68" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>127</v>
       </c>
       <c r="B69">
-        <v>9.9455869999999997</v>
+        <v>11.803749</v>
       </c>
       <c r="C69">
-        <v>-9.6966450000000002</v>
+        <v>-15.180413</v>
       </c>
       <c r="D69" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>129</v>
       </c>
       <c r="B70">
-        <v>11.803749</v>
+        <v>4.8604159999999998</v>
       </c>
       <c r="C70">
-        <v>-15.180413</v>
+        <v>-58.93018</v>
       </c>
       <c r="D70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>131</v>
       </c>
       <c r="B71">
-        <v>4.8604159999999998</v>
+        <v>18.971187</v>
       </c>
       <c r="C71">
-        <v>-58.93018</v>
+        <v>-72.285214999999994</v>
       </c>
       <c r="D71" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>352</v>
+      </c>
+      <c r="B72">
+        <v>41.902915999999998</v>
+      </c>
+      <c r="C72">
+        <v>12.453389</v>
+      </c>
+      <c r="D72" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>133</v>
       </c>
-      <c r="B72">
-        <v>18.971187</v>
-      </c>
-      <c r="C72">
-        <v>-72.285214999999994</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="B73">
+        <v>15.199999</v>
+      </c>
+      <c r="C73">
+        <v>-86.241905000000003</v>
+      </c>
+      <c r="D73" t="s">
         <v>134</v>
       </c>
-      <c r="E72" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>362</v>
-      </c>
-      <c r="B73">
-        <v>41.902915999999998</v>
-      </c>
-      <c r="C73">
-        <v>12.453389</v>
-      </c>
-      <c r="D73" t="s">
-        <v>358</v>
-      </c>
-      <c r="E73" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>135</v>
       </c>
       <c r="B74">
-        <v>15.199999</v>
+        <v>47.162494000000002</v>
       </c>
       <c r="C74">
-        <v>-86.241905000000003</v>
+        <v>19.503304</v>
       </c>
       <c r="D74" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>137</v>
       </c>
       <c r="B75">
-        <v>47.162494000000002</v>
+        <v>64.963050999999993</v>
       </c>
       <c r="C75">
-        <v>19.503304</v>
+        <v>-19.020835000000002</v>
       </c>
       <c r="D75" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>139</v>
       </c>
       <c r="B76">
-        <v>64.963050999999993</v>
+        <v>20.593684</v>
       </c>
       <c r="C76">
-        <v>-19.020835000000002</v>
+        <v>78.962879999999998</v>
       </c>
       <c r="D76" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>141</v>
       </c>
       <c r="B77">
-        <v>20.593684</v>
+        <v>-0.78927499999999995</v>
       </c>
       <c r="C77">
-        <v>78.962879999999998</v>
+        <v>113.92132700000001</v>
       </c>
       <c r="D77" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>143</v>
       </c>
       <c r="B78">
-        <v>-0.78927499999999995</v>
+        <v>32.427908000000002</v>
       </c>
       <c r="C78">
-        <v>113.92132700000001</v>
+        <v>53.688046</v>
       </c>
       <c r="D78" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="B79">
+        <v>33.223191</v>
+      </c>
+      <c r="C79">
+        <v>43.679290999999999</v>
+      </c>
+      <c r="D79" t="s">
         <v>145</v>
       </c>
-      <c r="B79">
-        <v>32.427908000000002</v>
-      </c>
-      <c r="C79">
-        <v>53.688046</v>
-      </c>
-      <c r="D79" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>146</v>
       </c>
       <c r="B80">
-        <v>33.223191</v>
+        <v>53.412909999999997</v>
       </c>
       <c r="C80">
-        <v>43.679290999999999</v>
+        <v>-8.2438900000000004</v>
       </c>
       <c r="D80" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>148</v>
       </c>
       <c r="B81">
-        <v>53.412909999999997</v>
+        <v>31.046050999999999</v>
       </c>
       <c r="C81">
-        <v>-8.2438900000000004</v>
+        <v>34.851612000000003</v>
       </c>
       <c r="D81" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>150</v>
       </c>
       <c r="B82">
-        <v>31.046050999999999</v>
+        <v>41.871940000000002</v>
       </c>
       <c r="C82">
-        <v>34.851612000000003</v>
+        <v>12.56738</v>
       </c>
       <c r="D82" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>152</v>
       </c>
       <c r="B83">
-        <v>41.871940000000002</v>
+        <v>18.109580999999999</v>
       </c>
       <c r="C83">
-        <v>12.56738</v>
+        <v>-77.297507999999993</v>
       </c>
       <c r="D83" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>154</v>
       </c>
       <c r="B84">
-        <v>18.109580999999999</v>
+        <v>36.204824000000002</v>
       </c>
       <c r="C84">
-        <v>-77.297507999999993</v>
+        <v>138.25292400000001</v>
       </c>
       <c r="D84" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>156</v>
       </c>
       <c r="B85">
-        <v>36.204824000000002</v>
+        <v>30.585163999999999</v>
       </c>
       <c r="C85">
-        <v>138.25292400000001</v>
+        <v>36.238413999999999</v>
       </c>
       <c r="D85" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>158</v>
       </c>
       <c r="B86">
-        <v>30.585163999999999</v>
+        <v>48.019573000000001</v>
       </c>
       <c r="C86">
-        <v>36.238413999999999</v>
+        <v>66.923683999999994</v>
       </c>
       <c r="D86" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>160</v>
       </c>
       <c r="B87">
-        <v>48.019573000000001</v>
+        <v>-2.3559E-2</v>
       </c>
       <c r="C87">
-        <v>66.923683999999994</v>
+        <v>37.906193000000002</v>
       </c>
       <c r="D87" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>162</v>
       </c>
       <c r="B88">
-        <v>-2.3559E-2</v>
+        <v>-3.3704170000000002</v>
       </c>
       <c r="C88">
-        <v>37.906193000000002</v>
+        <v>-168.734039</v>
       </c>
       <c r="D88" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>164</v>
       </c>
       <c r="B89">
-        <v>-3.3704170000000002</v>
+        <v>29.31166</v>
       </c>
       <c r="C89">
-        <v>-168.734039</v>
+        <v>47.481766</v>
       </c>
       <c r="D89" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>166</v>
       </c>
       <c r="B90">
-        <v>29.31166</v>
+        <v>41.20438</v>
       </c>
       <c r="C90">
-        <v>47.481766</v>
+        <v>74.766098</v>
       </c>
       <c r="D90" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>168</v>
-      </c>
       <c r="B91">
-        <v>41.20438</v>
+        <v>19.856269999999999</v>
       </c>
       <c r="C91">
-        <v>74.766098</v>
+        <v>102.495496</v>
       </c>
       <c r="D91" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92">
+        <v>56.879635</v>
+      </c>
+      <c r="C92">
+        <v>24.603189</v>
+      </c>
+      <c r="D92" t="s">
         <v>169</v>
       </c>
-      <c r="B92">
-        <v>19.856269999999999</v>
-      </c>
-      <c r="C92">
-        <v>102.495496</v>
-      </c>
-      <c r="D92" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>170</v>
       </c>
       <c r="B93">
-        <v>56.879635</v>
+        <v>33.854720999999998</v>
       </c>
       <c r="C93">
-        <v>24.603189</v>
+        <v>35.862285</v>
       </c>
       <c r="D93" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>172</v>
       </c>
       <c r="B94">
-        <v>33.854720999999998</v>
+        <v>-29.609988000000001</v>
       </c>
       <c r="C94">
-        <v>35.862285</v>
+        <v>28.233608</v>
       </c>
       <c r="D94" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>174</v>
       </c>
       <c r="B95">
-        <v>-29.609988000000001</v>
+        <v>6.4280549999999996</v>
       </c>
       <c r="C95">
-        <v>28.233608</v>
+        <v>-9.4294989999999999</v>
       </c>
       <c r="D95" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>176</v>
       </c>
       <c r="B96">
-        <v>6.4280549999999996</v>
+        <v>26.335100000000001</v>
       </c>
       <c r="C96">
-        <v>-9.4294989999999999</v>
+        <v>17.228331000000001</v>
       </c>
       <c r="D96" t="s">
         <v>177</v>
       </c>
-      <c r="E96" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>178</v>
       </c>
       <c r="B97">
-        <v>26.335100000000001</v>
+        <v>55.169438</v>
       </c>
       <c r="C97">
-        <v>17.228331000000001</v>
+        <v>23.881274999999999</v>
       </c>
       <c r="D97" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>180</v>
       </c>
       <c r="B98">
-        <v>47.165999999999997</v>
+        <v>49.815272999999998</v>
       </c>
       <c r="C98">
-        <v>9.5553729999999995</v>
+        <v>6.1295830000000002</v>
       </c>
       <c r="D98" t="s">
         <v>181</v>
       </c>
-      <c r="E98" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>182</v>
       </c>
       <c r="B99">
-        <v>55.169438</v>
+        <v>-18.766946999999998</v>
       </c>
       <c r="C99">
-        <v>23.881274999999999</v>
+        <v>46.869107</v>
       </c>
       <c r="D99" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>184</v>
       </c>
       <c r="B100">
-        <v>49.815272999999998</v>
+        <v>-13.254308</v>
       </c>
       <c r="C100">
-        <v>6.1295830000000002</v>
+        <v>34.301524999999998</v>
       </c>
       <c r="D100" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>186</v>
       </c>
       <c r="B101">
-        <v>-18.766946999999998</v>
+        <v>4.2104840000000001</v>
       </c>
       <c r="C101">
-        <v>46.869107</v>
+        <v>101.97576599999999</v>
       </c>
       <c r="D101" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>188</v>
       </c>
       <c r="B102">
-        <v>-13.254308</v>
+        <v>3.2027779999999999</v>
       </c>
       <c r="C102">
-        <v>34.301524999999998</v>
+        <v>73.220680000000002</v>
       </c>
       <c r="D102" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>190</v>
       </c>
       <c r="B103">
-        <v>4.2104840000000001</v>
+        <v>17.570692000000001</v>
       </c>
       <c r="C103">
-        <v>101.97576599999999</v>
+        <v>-3.9961660000000001</v>
       </c>
       <c r="D103" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>192</v>
       </c>
       <c r="B104">
-        <v>3.2027779999999999</v>
+        <v>35.937496000000003</v>
       </c>
       <c r="C104">
-        <v>73.220680000000002</v>
+        <v>14.375416</v>
       </c>
       <c r="D104" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>194</v>
       </c>
       <c r="B105">
-        <v>17.570692000000001</v>
+        <v>7.1314739999999999</v>
       </c>
       <c r="C105">
-        <v>-3.9961660000000001</v>
+        <v>171.18447800000001</v>
       </c>
       <c r="D105" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>196</v>
       </c>
       <c r="B106">
-        <v>35.937496000000003</v>
+        <v>21.00789</v>
       </c>
       <c r="C106">
-        <v>14.375416</v>
+        <v>-10.940835</v>
       </c>
       <c r="D106" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>198</v>
       </c>
       <c r="B107">
-        <v>7.1314739999999999</v>
+        <v>-20.348403999999999</v>
       </c>
       <c r="C107">
-        <v>171.18447800000001</v>
+        <v>57.552152</v>
       </c>
       <c r="D107" t="s">
         <v>199</v>
       </c>
-      <c r="E107" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>200</v>
       </c>
       <c r="B108">
-        <v>21.00789</v>
+        <v>23.634501</v>
       </c>
       <c r="C108">
-        <v>-10.940835</v>
+        <v>-102.552784</v>
       </c>
       <c r="D108" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>202</v>
       </c>
       <c r="B109">
-        <v>-20.348403999999999</v>
+        <v>7.425554</v>
       </c>
       <c r="C109">
-        <v>57.552152</v>
+        <v>150.55081200000001</v>
       </c>
       <c r="D109" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="B110">
+        <v>47.411631</v>
+      </c>
+      <c r="C110">
+        <v>28.369885</v>
+      </c>
+      <c r="D110" t="s">
         <v>204</v>
       </c>
-      <c r="B110">
-        <v>23.634501</v>
-      </c>
-      <c r="C110">
-        <v>-102.552784</v>
-      </c>
-      <c r="D110" t="s">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="B111">
+        <v>46.862496</v>
+      </c>
+      <c r="C111">
+        <v>103.846656</v>
+      </c>
+      <c r="D111" t="s">
         <v>206</v>
       </c>
-      <c r="B111">
-        <v>7.425554</v>
-      </c>
-      <c r="C111">
-        <v>150.55081200000001</v>
-      </c>
-      <c r="D111" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>207</v>
       </c>
       <c r="B112">
-        <v>47.411631</v>
+        <v>42.708677999999999</v>
       </c>
       <c r="C112">
-        <v>28.369885</v>
+        <v>19.374389999999998</v>
       </c>
       <c r="D112" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>209</v>
       </c>
       <c r="B113">
-        <v>43.750298000000001</v>
+        <v>31.791702000000001</v>
       </c>
       <c r="C113">
-        <v>7.4128410000000002</v>
+        <v>-7.0926200000000001</v>
       </c>
       <c r="D113" t="s">
         <v>210</v>
       </c>
-      <c r="E113" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>211</v>
       </c>
       <c r="B114">
-        <v>46.862496</v>
+        <v>-18.665694999999999</v>
       </c>
       <c r="C114">
-        <v>103.846656</v>
+        <v>35.529561999999999</v>
       </c>
       <c r="D114" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>213</v>
       </c>
       <c r="B115">
-        <v>42.708677999999999</v>
+        <v>21.913965000000001</v>
       </c>
       <c r="C115">
-        <v>19.374389999999998</v>
+        <v>95.956222999999994</v>
       </c>
       <c r="D115" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="B116">
+        <v>-22.957640000000001</v>
+      </c>
+      <c r="C116">
+        <v>18.490410000000001</v>
+      </c>
+      <c r="D116" t="s">
         <v>215</v>
       </c>
-      <c r="B116">
-        <v>31.791702000000001</v>
-      </c>
-      <c r="C116">
-        <v>-7.0926200000000001</v>
-      </c>
-      <c r="D116" t="s">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="B117">
+        <v>-0.52277799999999996</v>
+      </c>
+      <c r="C117">
+        <v>166.93150299999999</v>
+      </c>
+      <c r="D117" t="s">
         <v>217</v>
       </c>
-      <c r="B117">
-        <v>-18.665694999999999</v>
-      </c>
-      <c r="C117">
-        <v>35.529561999999999</v>
-      </c>
-      <c r="D117" t="s">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B118">
+        <v>28.394856999999998</v>
+      </c>
+      <c r="C118">
+        <v>84.124008000000003</v>
+      </c>
+      <c r="D118" t="s">
         <v>219</v>
       </c>
-      <c r="B118">
-        <v>21.913965000000001</v>
-      </c>
-      <c r="C118">
-        <v>95.956222999999994</v>
-      </c>
-      <c r="D118" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>220</v>
       </c>
       <c r="B119">
-        <v>-22.957640000000001</v>
+        <v>52.132632999999998</v>
       </c>
       <c r="C119">
-        <v>18.490410000000001</v>
+        <v>5.2912660000000002</v>
       </c>
       <c r="D119" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>222</v>
       </c>
       <c r="B120">
-        <v>-0.52277799999999996</v>
+        <v>-40.900556999999999</v>
       </c>
       <c r="C120">
-        <v>166.93150299999999</v>
+        <v>174.88597100000001</v>
       </c>
       <c r="D120" t="s">
         <v>223</v>
       </c>
-      <c r="E120" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>224</v>
       </c>
       <c r="B121">
-        <v>28.394856999999998</v>
+        <v>12.865416</v>
       </c>
       <c r="C121">
-        <v>84.124008000000003</v>
+        <v>-85.207228999999998</v>
       </c>
       <c r="D121" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>226</v>
       </c>
       <c r="B122">
-        <v>52.132632999999998</v>
+        <v>17.607789</v>
       </c>
       <c r="C122">
-        <v>5.2912660000000002</v>
+        <v>8.0816660000000002</v>
       </c>
       <c r="D122" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>228</v>
       </c>
       <c r="B123">
-        <v>-40.900556999999999</v>
+        <v>9.0819989999999997</v>
       </c>
       <c r="C123">
-        <v>174.88597100000001</v>
+        <v>8.6752769999999995</v>
       </c>
       <c r="D123" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>230</v>
       </c>
       <c r="B124">
-        <v>12.865416</v>
+        <v>60.472023999999998</v>
       </c>
       <c r="C124">
-        <v>-85.207228999999998</v>
+        <v>8.4689460000000008</v>
       </c>
       <c r="D124" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>232</v>
       </c>
       <c r="B125">
-        <v>17.607789</v>
+        <v>21.512582999999999</v>
       </c>
       <c r="C125">
-        <v>8.0816660000000002</v>
+        <v>55.923254999999997</v>
       </c>
       <c r="D125" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>234</v>
       </c>
       <c r="B126">
-        <v>9.0819989999999997</v>
+        <v>30.375321</v>
       </c>
       <c r="C126">
-        <v>8.6752769999999995</v>
+        <v>69.345116000000004</v>
       </c>
       <c r="D126" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>236</v>
       </c>
       <c r="B127">
-        <v>40.339852</v>
+        <v>7.5149800000000004</v>
       </c>
       <c r="C127">
-        <v>127.510093</v>
+        <v>134.58251999999999</v>
       </c>
       <c r="D127" t="s">
         <v>237</v>
       </c>
-      <c r="E127" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>238</v>
       </c>
       <c r="B128">
-        <v>60.472023999999998</v>
+        <v>8.5379810000000003</v>
       </c>
       <c r="C128">
-        <v>8.4689460000000008</v>
+        <v>-80.782127000000003</v>
       </c>
       <c r="D128" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>240</v>
       </c>
       <c r="B129">
-        <v>21.512582999999999</v>
+        <v>-6.3149930000000003</v>
       </c>
       <c r="C129">
-        <v>55.923254999999997</v>
+        <v>143.95554999999999</v>
       </c>
       <c r="D129" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>242</v>
       </c>
       <c r="B130">
-        <v>30.375321</v>
+        <v>-23.442502999999999</v>
       </c>
       <c r="C130">
-        <v>69.345116000000004</v>
+        <v>-58.443832</v>
       </c>
       <c r="D130" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>244</v>
       </c>
       <c r="B131">
-        <v>7.5149800000000004</v>
+        <v>-9.1899669999999993</v>
       </c>
       <c r="C131">
-        <v>134.58251999999999</v>
+        <v>-75.015152</v>
       </c>
       <c r="D131" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>246</v>
       </c>
       <c r="B132">
-        <v>8.5379810000000003</v>
+        <v>12.879721</v>
       </c>
       <c r="C132">
-        <v>-80.782127000000003</v>
+        <v>121.774017</v>
       </c>
       <c r="D132" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>248</v>
       </c>
       <c r="B133">
-        <v>-6.3149930000000003</v>
+        <v>51.919438</v>
       </c>
       <c r="C133">
-        <v>143.95554999999999</v>
+        <v>19.145136000000001</v>
       </c>
       <c r="D133" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>250</v>
       </c>
       <c r="B134">
-        <v>-23.442502999999999</v>
+        <v>39.399872000000002</v>
       </c>
       <c r="C134">
-        <v>-58.443832</v>
+        <v>-8.2244539999999997</v>
       </c>
       <c r="D134" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>252</v>
       </c>
       <c r="B135">
-        <v>-9.1899669999999993</v>
+        <v>25.354825999999999</v>
       </c>
       <c r="C135">
-        <v>-75.015152</v>
+        <v>51.183883999999999</v>
       </c>
       <c r="D135" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>254</v>
       </c>
       <c r="B136">
-        <v>12.879721</v>
+        <v>45.943161000000003</v>
       </c>
       <c r="C136">
-        <v>121.774017</v>
+        <v>24.966760000000001</v>
       </c>
       <c r="D136" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>256</v>
       </c>
       <c r="B137">
-        <v>51.919438</v>
+        <v>61.524009999999997</v>
       </c>
       <c r="C137">
-        <v>19.145136000000001</v>
+        <v>105.31875599999999</v>
       </c>
       <c r="D137" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="B138">
+        <v>-1.9402779999999999</v>
+      </c>
+      <c r="C138">
+        <v>29.873888000000001</v>
+      </c>
+      <c r="D138" t="s">
         <v>258</v>
       </c>
-      <c r="B138">
-        <v>39.399872000000002</v>
-      </c>
-      <c r="C138">
-        <v>-8.2244539999999997</v>
-      </c>
-      <c r="D138" t="s">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="B139">
+        <v>17.357821999999999</v>
+      </c>
+      <c r="C139">
+        <v>-62.782997999999999</v>
+      </c>
+      <c r="D139" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>260</v>
       </c>
-      <c r="B139">
-        <v>25.354825999999999</v>
-      </c>
-      <c r="C139">
-        <v>51.183883999999999</v>
-      </c>
-      <c r="D139" t="s">
+      <c r="B140">
+        <v>13.909444000000001</v>
+      </c>
+      <c r="C140">
+        <v>-60.978892999999999</v>
+      </c>
+      <c r="D140" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="B141">
+        <v>-13.759029</v>
+      </c>
+      <c r="C141">
+        <v>-172.10462899999999</v>
+      </c>
+      <c r="D141" t="s">
         <v>262</v>
       </c>
-      <c r="B140">
-        <v>45.943161000000003</v>
-      </c>
-      <c r="C140">
-        <v>24.966760000000001</v>
-      </c>
-      <c r="D140" t="s">
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="B142">
+        <v>43.942360000000001</v>
+      </c>
+      <c r="C142">
+        <v>12.457777</v>
+      </c>
+      <c r="D142" t="s">
         <v>264</v>
       </c>
-      <c r="B141">
-        <v>61.524009999999997</v>
-      </c>
-      <c r="C141">
-        <v>105.31875599999999</v>
-      </c>
-      <c r="D141" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>265</v>
       </c>
-      <c r="B142">
-        <v>-1.9402779999999999</v>
-      </c>
-      <c r="C142">
-        <v>29.873888000000001</v>
-      </c>
-      <c r="D142" t="s">
+      <c r="B143">
+        <v>0.18636</v>
+      </c>
+      <c r="C143">
+        <v>6.6130810000000002</v>
+      </c>
+      <c r="D143" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="B144">
+        <v>23.885942</v>
+      </c>
+      <c r="C144">
+        <v>45.079161999999997</v>
+      </c>
+      <c r="D144" t="s">
         <v>267</v>
       </c>
-      <c r="B143">
-        <v>17.357821999999999</v>
-      </c>
-      <c r="C143">
-        <v>-62.782997999999999</v>
-      </c>
-      <c r="D143" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>268</v>
       </c>
-      <c r="B144">
-        <v>13.909444000000001</v>
-      </c>
-      <c r="C144">
-        <v>-60.978892999999999</v>
-      </c>
-      <c r="D144" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="B145">
+        <v>14.497401</v>
+      </c>
+      <c r="C145">
+        <v>-14.452362000000001</v>
+      </c>
+      <c r="D145" t="s">
         <v>269</v>
       </c>
-      <c r="B145">
-        <v>-13.759029</v>
-      </c>
-      <c r="C145">
-        <v>-172.10462899999999</v>
-      </c>
-      <c r="D145" t="s">
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="B146">
+        <v>-4.6795739999999997</v>
+      </c>
+      <c r="C146">
+        <v>55.491976999999999</v>
+      </c>
+      <c r="D146" t="s">
         <v>271</v>
       </c>
-      <c r="B146">
-        <v>43.942360000000001</v>
-      </c>
-      <c r="C146">
-        <v>12.457777</v>
-      </c>
-      <c r="D146" t="s">
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>272</v>
       </c>
-      <c r="E146" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="B147">
+        <v>8.4605549999999994</v>
+      </c>
+      <c r="C147">
+        <v>-11.779889000000001</v>
+      </c>
+      <c r="D147" t="s">
         <v>273</v>
       </c>
-      <c r="B147">
-        <v>0.18636</v>
-      </c>
-      <c r="C147">
-        <v>6.6130810000000002</v>
-      </c>
-      <c r="D147" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>274</v>
       </c>
       <c r="B148">
-        <v>23.885942</v>
+        <v>1.3520829999999999</v>
       </c>
       <c r="C148">
-        <v>45.079161999999997</v>
+        <v>103.819836</v>
       </c>
       <c r="D148" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>276</v>
       </c>
       <c r="B149">
-        <v>14.497401</v>
+        <v>48.669026000000002</v>
       </c>
       <c r="C149">
-        <v>-14.452362000000001</v>
+        <v>19.699024000000001</v>
       </c>
       <c r="D149" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="B150">
+        <v>46.151240999999999</v>
+      </c>
+      <c r="C150">
+        <v>14.995463000000001</v>
+      </c>
+      <c r="D150" t="s">
         <v>278</v>
       </c>
-      <c r="B150">
-        <v>44.016520999999997</v>
-      </c>
-      <c r="C150">
-        <v>21.005859000000001</v>
-      </c>
-      <c r="D150" t="s">
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>279</v>
       </c>
-      <c r="E150" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="B151">
+        <v>-9.6457099999999993</v>
+      </c>
+      <c r="C151">
+        <v>160.156194</v>
+      </c>
+      <c r="D151" t="s">
         <v>280</v>
       </c>
-      <c r="B151">
-        <v>-4.6795739999999997</v>
-      </c>
-      <c r="C151">
-        <v>55.491976999999999</v>
-      </c>
-      <c r="D151" t="s">
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="B152">
+        <v>5.1521489999999996</v>
+      </c>
+      <c r="C152">
+        <v>46.199615999999999</v>
+      </c>
+      <c r="D152" t="s">
         <v>282</v>
       </c>
-      <c r="B152">
-        <v>8.4605549999999994</v>
-      </c>
-      <c r="C152">
-        <v>-11.779889000000001</v>
-      </c>
-      <c r="D152" t="s">
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="B153">
+        <v>-30.559481999999999</v>
+      </c>
+      <c r="C153">
+        <v>22.937505999999999</v>
+      </c>
+      <c r="D153" t="s">
         <v>284</v>
       </c>
-      <c r="B153">
-        <v>1.3520829999999999</v>
-      </c>
-      <c r="C153">
-        <v>103.819836</v>
-      </c>
-      <c r="D153" t="s">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="B154">
+        <v>35.907756999999997</v>
+      </c>
+      <c r="C154">
+        <v>127.76692199999999</v>
+      </c>
+      <c r="D154" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>353</v>
+      </c>
+      <c r="B155">
+        <v>4.8593630000000001</v>
+      </c>
+      <c r="C155">
+        <v>31.571251</v>
+      </c>
+      <c r="D155" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>286</v>
       </c>
-      <c r="B154">
-        <v>48.669026000000002</v>
-      </c>
-      <c r="C154">
-        <v>19.699024000000001</v>
-      </c>
-      <c r="D154" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="B156">
+        <v>40.463667000000001</v>
+      </c>
+      <c r="C156">
+        <v>-3.7492200000000002</v>
+      </c>
+      <c r="D156" t="s">
         <v>287</v>
       </c>
-      <c r="B155">
-        <v>46.151240999999999</v>
-      </c>
-      <c r="C155">
-        <v>14.995463000000001</v>
-      </c>
-      <c r="D155" t="s">
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="B157">
+        <v>7.8730539999999998</v>
+      </c>
+      <c r="C157">
+        <v>80.771797000000007</v>
+      </c>
+      <c r="D157" t="s">
         <v>289</v>
       </c>
-      <c r="B156">
-        <v>-9.6457099999999993</v>
-      </c>
-      <c r="C156">
-        <v>160.156194</v>
-      </c>
-      <c r="D156" t="s">
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>354</v>
+      </c>
+      <c r="B158">
+        <v>12.984305000000001</v>
+      </c>
+      <c r="C158">
+        <v>-61.287227999999999</v>
+      </c>
+      <c r="D158" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>355</v>
+      </c>
+      <c r="B159">
+        <v>31.952162000000001</v>
+      </c>
+      <c r="C159">
+        <v>35.233153999999999</v>
+      </c>
+      <c r="D159" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="B160">
+        <v>12.862807</v>
+      </c>
+      <c r="C160">
+        <v>30.217635999999999</v>
+      </c>
+      <c r="D160" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>291</v>
       </c>
-      <c r="B157">
-        <v>5.1521489999999996</v>
-      </c>
-      <c r="C157">
-        <v>46.199615999999999</v>
-      </c>
-      <c r="D157" t="s">
+      <c r="B161">
+        <v>3.919305</v>
+      </c>
+      <c r="C161">
+        <v>-56.027782999999999</v>
+      </c>
+      <c r="D161" t="s">
         <v>292</v>
       </c>
-      <c r="E157" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>293</v>
       </c>
-      <c r="B158">
-        <v>-30.559481999999999</v>
-      </c>
-      <c r="C158">
-        <v>22.937505999999999</v>
-      </c>
-      <c r="D158" t="s">
+      <c r="B162">
+        <v>-26.522503</v>
+      </c>
+      <c r="C162">
+        <v>31.465865999999998</v>
+      </c>
+      <c r="D162" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>295</v>
       </c>
-      <c r="B159">
-        <v>35.907756999999997</v>
-      </c>
-      <c r="C159">
-        <v>127.76692199999999</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="B163">
+        <v>60.128160999999999</v>
+      </c>
+      <c r="C163">
+        <v>18.643501000000001</v>
+      </c>
+      <c r="D163" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>297</v>
+      </c>
+      <c r="B164">
+        <v>46.818187999999999</v>
+      </c>
+      <c r="C164">
+        <v>8.2275120000000008</v>
+      </c>
+      <c r="D164" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>299</v>
+      </c>
+      <c r="B165">
+        <v>34.802075000000002</v>
+      </c>
+      <c r="C165">
+        <v>38.996814999999998</v>
+      </c>
+      <c r="D165" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>300</v>
+      </c>
+      <c r="B166">
+        <v>38.861033999999997</v>
+      </c>
+      <c r="C166">
+        <v>71.276093000000003</v>
+      </c>
+      <c r="D166" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>302</v>
+      </c>
+      <c r="B167">
+        <v>-6.3690280000000001</v>
+      </c>
+      <c r="C167">
+        <v>34.888821999999998</v>
+      </c>
+      <c r="D167" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>350</v>
+      </c>
+      <c r="B168">
+        <v>41.608635</v>
+      </c>
+      <c r="C168">
+        <v>21.745274999999999</v>
+      </c>
+      <c r="D168" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>363</v>
-      </c>
-      <c r="B160">
-        <v>4.8593630000000001</v>
-      </c>
-      <c r="C160">
-        <v>31.571251</v>
-      </c>
-      <c r="D160" t="s">
-        <v>359</v>
-      </c>
-      <c r="E160" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>296</v>
-      </c>
-      <c r="B161">
-        <v>40.463667000000001</v>
-      </c>
-      <c r="C161">
-        <v>-3.7492200000000002</v>
-      </c>
-      <c r="D161" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>298</v>
-      </c>
-      <c r="B162">
-        <v>7.8730539999999998</v>
-      </c>
-      <c r="C162">
-        <v>80.771797000000007</v>
-      </c>
-      <c r="D162" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>364</v>
-      </c>
-      <c r="B163">
-        <v>12.984305000000001</v>
-      </c>
-      <c r="C163">
-        <v>-61.287227999999999</v>
-      </c>
-      <c r="D163" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>365</v>
-      </c>
-      <c r="B164">
-        <v>31.952162000000001</v>
-      </c>
-      <c r="C164">
-        <v>35.233153999999999</v>
-      </c>
-      <c r="D164" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>300</v>
-      </c>
-      <c r="B165">
-        <v>12.862807</v>
-      </c>
-      <c r="C165">
-        <v>30.217635999999999</v>
-      </c>
-      <c r="D165" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>301</v>
-      </c>
-      <c r="B166">
-        <v>3.919305</v>
-      </c>
-      <c r="C166">
-        <v>-56.027782999999999</v>
-      </c>
-      <c r="D166" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>303</v>
-      </c>
-      <c r="B167">
-        <v>-26.522503</v>
-      </c>
-      <c r="C167">
-        <v>31.465865999999998</v>
-      </c>
-      <c r="D167" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+      <c r="B169">
+        <v>15.870032</v>
+      </c>
+      <c r="C169">
+        <v>100.992541</v>
+      </c>
+      <c r="D169" t="s">
         <v>305</v>
       </c>
-      <c r="B168">
-        <v>60.128160999999999</v>
-      </c>
-      <c r="C168">
-        <v>18.643501000000001</v>
-      </c>
-      <c r="D168" t="s">
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="B170">
+        <v>-8.8742169999999998</v>
+      </c>
+      <c r="C170">
+        <v>125.72753899999999</v>
+      </c>
+      <c r="D170" t="s">
         <v>307</v>
       </c>
-      <c r="B169">
-        <v>46.818187999999999</v>
-      </c>
-      <c r="C169">
-        <v>8.2275120000000008</v>
-      </c>
-      <c r="D169" t="s">
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+      <c r="B171">
+        <v>8.6195430000000002</v>
+      </c>
+      <c r="C171">
+        <v>0.82478200000000002</v>
+      </c>
+      <c r="D171" t="s">
         <v>309</v>
       </c>
-      <c r="B170">
-        <v>34.802075000000002</v>
-      </c>
-      <c r="C170">
-        <v>38.996814999999998</v>
-      </c>
-      <c r="D170" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>310</v>
       </c>
-      <c r="B171">
-        <v>38.861033999999997</v>
-      </c>
-      <c r="C171">
-        <v>71.276093000000003</v>
-      </c>
-      <c r="D171" t="s">
+      <c r="B172">
+        <v>-21.178985999999998</v>
+      </c>
+      <c r="C172">
+        <v>-175.19824199999999</v>
+      </c>
+      <c r="D172" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>312</v>
       </c>
-      <c r="B172">
-        <v>-6.3690280000000001</v>
-      </c>
-      <c r="C172">
-        <v>34.888821999999998</v>
-      </c>
-      <c r="D172" t="s">
+      <c r="B173">
+        <v>10.691803</v>
+      </c>
+      <c r="C173">
+        <v>-61.222503000000003</v>
+      </c>
+      <c r="D173" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>360</v>
-      </c>
-      <c r="B173">
-        <v>41.608635</v>
-      </c>
-      <c r="C173">
-        <v>21.745274999999999</v>
-      </c>
-      <c r="D173" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>314</v>
       </c>
       <c r="B174">
-        <v>15.870032</v>
+        <v>33.886916999999997</v>
       </c>
       <c r="C174">
-        <v>100.992541</v>
+        <v>9.5374990000000004</v>
       </c>
       <c r="D174" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>316</v>
       </c>
       <c r="B175">
-        <v>-8.8742169999999998</v>
+        <v>38.963745000000003</v>
       </c>
       <c r="C175">
-        <v>125.72753899999999</v>
+        <v>35.243321999999999</v>
       </c>
       <c r="D175" t="s">
         <v>317</v>
       </c>
-      <c r="E175" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>318</v>
       </c>
       <c r="B176">
-        <v>8.6195430000000002</v>
+        <v>38.969718999999998</v>
       </c>
       <c r="C176">
-        <v>0.82478200000000002</v>
+        <v>59.556277999999999</v>
       </c>
       <c r="D176" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>320</v>
       </c>
       <c r="B177">
-        <v>-21.178985999999998</v>
+        <v>-7.1095350000000002</v>
       </c>
       <c r="C177">
-        <v>-175.19824199999999</v>
+        <v>177.64932999999999</v>
       </c>
       <c r="D177" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>322</v>
       </c>
       <c r="B178">
-        <v>10.691803</v>
+        <v>1.3733329999999999</v>
       </c>
       <c r="C178">
-        <v>-61.222503000000003</v>
+        <v>32.290275000000001</v>
       </c>
       <c r="D178" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>324</v>
       </c>
       <c r="B179">
-        <v>33.886916999999997</v>
+        <v>48.379432999999999</v>
       </c>
       <c r="C179">
-        <v>9.5374990000000004</v>
+        <v>31.165579999999999</v>
       </c>
       <c r="D179" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>326</v>
       </c>
       <c r="B180">
-        <v>38.963745000000003</v>
+        <v>23.424075999999999</v>
       </c>
       <c r="C180">
-        <v>35.243321999999999</v>
+        <v>53.847817999999997</v>
       </c>
       <c r="D180" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>328</v>
       </c>
       <c r="B181">
-        <v>38.969718999999998</v>
+        <v>55.378050999999999</v>
       </c>
       <c r="C181">
-        <v>59.556277999999999</v>
+        <v>-3.4359730000000002</v>
       </c>
       <c r="D181" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>330</v>
       </c>
       <c r="B182">
-        <v>-7.1095350000000002</v>
+        <v>37.090240000000001</v>
       </c>
       <c r="C182">
-        <v>177.64932999999999</v>
+        <v>-95.712890999999999</v>
       </c>
       <c r="D182" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>332</v>
       </c>
       <c r="B183">
-        <v>1.3733329999999999</v>
+        <v>-32.522779</v>
       </c>
       <c r="C183">
-        <v>32.290275000000001</v>
+        <v>-55.765835000000003</v>
       </c>
       <c r="D183" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>334</v>
       </c>
       <c r="B184">
-        <v>48.379432999999999</v>
+        <v>41.377490999999999</v>
       </c>
       <c r="C184">
-        <v>31.165579999999999</v>
+        <v>64.585262</v>
       </c>
       <c r="D184" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>336</v>
       </c>
       <c r="B185">
-        <v>23.424075999999999</v>
+        <v>-15.376706</v>
       </c>
       <c r="C185">
-        <v>53.847817999999997</v>
+        <v>166.959158</v>
       </c>
       <c r="D185" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>338</v>
       </c>
       <c r="B186">
-        <v>55.378050999999999</v>
+        <v>6.4237500000000001</v>
       </c>
       <c r="C186">
-        <v>-3.4359730000000002</v>
+        <v>-66.589730000000003</v>
       </c>
       <c r="D186" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>340</v>
       </c>
       <c r="B187">
-        <v>37.090240000000001</v>
+        <v>14.058324000000001</v>
       </c>
       <c r="C187">
-        <v>-95.712890999999999</v>
+        <v>108.277199</v>
       </c>
       <c r="D187" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>342</v>
       </c>
       <c r="B188">
-        <v>-32.522779</v>
+        <v>15.552727000000001</v>
       </c>
       <c r="C188">
-        <v>-55.765835000000003</v>
+        <v>48.516387999999999</v>
       </c>
       <c r="D188" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>344</v>
       </c>
       <c r="B189">
-        <v>41.377490999999999</v>
+        <v>-13.133896999999999</v>
       </c>
       <c r="C189">
-        <v>64.585262</v>
+        <v>27.849332</v>
       </c>
       <c r="D189" t="s">
         <v>345</v>
       </c>
-      <c r="E189" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>346</v>
       </c>
       <c r="B190">
-        <v>-15.376706</v>
+        <v>-19.015438</v>
       </c>
       <c r="C190">
-        <v>166.959158</v>
+        <v>29.154857</v>
       </c>
       <c r="D190" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>348</v>
-      </c>
-      <c r="B191">
-        <v>6.4237500000000001</v>
-      </c>
-      <c r="C191">
-        <v>-66.589730000000003</v>
-      </c>
-      <c r="D191" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>350</v>
-      </c>
-      <c r="B192">
-        <v>14.058324000000001</v>
-      </c>
-      <c r="C192">
-        <v>108.277199</v>
-      </c>
-      <c r="D192" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>352</v>
-      </c>
-      <c r="B193">
-        <v>15.552727000000001</v>
-      </c>
-      <c r="C193">
-        <v>48.516387999999999</v>
-      </c>
-      <c r="D193" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>354</v>
-      </c>
-      <c r="B194">
-        <v>-13.133896999999999</v>
-      </c>
-      <c r="C194">
-        <v>27.849332</v>
-      </c>
-      <c r="D194" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>356</v>
-      </c>
-      <c r="B195">
-        <v>-19.015438</v>
-      </c>
-      <c r="C195">
-        <v>29.154857</v>
-      </c>
-      <c r="D195" t="s">
-        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>